<commit_message>
Set things up so that I can test/edit SampleConfig direct from repo folder (so I don't have to keep copying files around).
</commit_message>
<xml_diff>
--- a/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
+++ b/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csudbery/ReconciliateCsvs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\ManualTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC415C8-4329-A84C-BBD6-0F7DE871DFDE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720D0FA9-E33C-4B1A-BFF5-CE82B40C5CF1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25680" yWindow="8980" windowWidth="25600" windowHeight="8940" activeTab="10" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank In" sheetId="7" r:id="rId1"/>
@@ -633,8 +633,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
@@ -710,18 +710,18 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -729,7 +729,7 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -740,10 +740,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -753,30 +753,30 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1203,19 +1203,19 @@
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.83203125" customWidth="1"/>
-    <col min="5" max="5" width="30.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.85546875" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>43586</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>43587</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>43588</v>
       </c>
@@ -1339,13 +1339,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>43616</v>
       </c>
@@ -1380,15 +1380,15 @@
       <selection pane="bottomLeft" activeCell="F2" sqref="F2:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="45" t="s">
         <v>21</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>10</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>11</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>12</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="49" t="s">
         <v>108</v>
       </c>
@@ -1493,23 +1493,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF22F54-1C2B-49C1-90A9-21044AC295B0}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>21</v>
       </c>
@@ -1534,7 +1535,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="34" t="s">
         <v>72</v>
       </c>
@@ -1542,7 +1543,7 @@
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
     </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>26</v>
       </c>
@@ -1561,7 +1562,7 @@
       </c>
       <c r="K3" s="20"/>
     </row>
-    <row r="4" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>27</v>
       </c>
@@ -1580,7 +1581,7 @@
       </c>
       <c r="K4" s="20"/>
     </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>86</v>
       </c>
@@ -1598,7 +1599,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="16" t="s">
         <v>73</v>
       </c>
@@ -1610,14 +1611,14 @@
       <c r="E6" s="17"/>
       <c r="F6" s="19"/>
     </row>
-    <row r="7" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="16"/>
       <c r="C7" s="18"/>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
       <c r="F7" s="19"/>
     </row>
-    <row r="8" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="15" t="s">
         <v>74</v>
       </c>
@@ -1626,7 +1627,7 @@
       <c r="E8" s="17"/>
       <c r="F8" s="19"/>
     </row>
-    <row r="9" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>87</v>
       </c>
@@ -1650,7 +1651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>88</v>
       </c>
@@ -1672,7 +1673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>89</v>
       </c>
@@ -1693,7 +1694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>120</v>
       </c>
@@ -1714,7 +1715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B13" s="46" t="s">
         <v>75</v>
       </c>
@@ -1723,7 +1724,7 @@
       <c r="E13" s="17"/>
       <c r="F13" s="19"/>
     </row>
-    <row r="14" spans="1:12" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>90</v>
       </c>
@@ -1741,7 +1742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>91</v>
       </c>
@@ -1759,7 +1760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>92</v>
       </c>
@@ -1777,13 +1778,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="46" t="s">
         <v>76</v>
       </c>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>93</v>
       </c>
@@ -1808,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>94</v>
       </c>
@@ -1833,7 +1834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>95</v>
       </c>
@@ -1858,7 +1859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21" s="45" t="s">
         <v>77</v>
       </c>
@@ -1867,15 +1868,15 @@
         <v>1675</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" s="34" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>96</v>
       </c>
@@ -1899,7 +1900,7 @@
       <c r="K24" s="20"/>
       <c r="L24" s="14"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>97</v>
       </c>
@@ -1923,7 +1924,7 @@
       <c r="K25" s="20"/>
       <c r="L25" s="14"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>98</v>
       </c>
@@ -1947,7 +1948,7 @@
       <c r="K26" s="14"/>
       <c r="L26" s="14"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" s="47" t="s">
         <v>79</v>
       </c>
@@ -1966,24 +1967,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C703CDFE-5895-4A70-B218-454B4A08CC66}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O7" sqref="O7"/>
+      <selection pane="bottomLeft" activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.83203125" customWidth="1"/>
-    <col min="5" max="5" width="30.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.85546875" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -2003,7 +2004,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>43586</v>
       </c>
@@ -2037,7 +2038,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>43587</v>
       </c>
@@ -2071,7 +2072,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>43588</v>
       </c>
@@ -2107,7 +2108,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>43589</v>
       </c>
@@ -2141,7 +2142,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>43597</v>
       </c>
@@ -2175,7 +2176,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>43598</v>
       </c>
@@ -2209,12 +2210,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>43616</v>
       </c>
@@ -2249,18 +2250,18 @@
       <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.1640625" customWidth="1"/>
-    <col min="4" max="4" width="30.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.140625" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>1</v>
       </c>
@@ -2278,7 +2279,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>43586</v>
       </c>
@@ -2302,7 +2303,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>43587</v>
       </c>
@@ -2326,7 +2327,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>43588</v>
       </c>
@@ -2350,13 +2351,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="38" t="s">
         <v>9</v>
       </c>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>43616</v>
       </c>
@@ -2383,18 +2384,18 @@
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.1640625" customWidth="1"/>
-    <col min="4" max="4" width="30.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.140625" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>1</v>
       </c>
@@ -2412,7 +2413,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>43586</v>
       </c>
@@ -2436,7 +2437,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>43587</v>
       </c>
@@ -2460,7 +2461,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>43588</v>
       </c>
@@ -2484,13 +2485,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="38" t="s">
         <v>9</v>
       </c>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>43616</v>
       </c>
@@ -2517,18 +2518,18 @@
       <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="34" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" s="34" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
         <v>1</v>
       </c>
@@ -2555,7 +2556,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>43586</v>
       </c>
@@ -2572,7 +2573,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>43587</v>
       </c>
@@ -2592,7 +2593,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>43588</v>
       </c>
@@ -2612,12 +2613,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>43617</v>
       </c>
@@ -2631,7 +2632,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>43618</v>
       </c>
@@ -2645,7 +2646,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>43619</v>
       </c>
@@ -2673,15 +2674,15 @@
       <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>21</v>
       </c>
@@ -2699,7 +2700,7 @@
       <c r="H1" s="23"/>
       <c r="I1" s="23"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
@@ -2716,7 +2717,7 @@
       <c r="H2" s="26"/>
       <c r="I2" s="26"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="28"/>
       <c r="B3" s="25"/>
       <c r="C3" s="26"/>
@@ -2729,7 +2730,7 @@
       <c r="H3" s="26"/>
       <c r="I3" s="26"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>11</v>
       </c>
@@ -2746,7 +2747,7 @@
       <c r="H4" s="26"/>
       <c r="I4" s="26"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>12</v>
       </c>
@@ -2763,7 +2764,7 @@
       <c r="H5" s="26"/>
       <c r="I5" s="26"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="28"/>
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
@@ -2776,7 +2777,7 @@
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="28"/>
       <c r="B7" s="25">
         <v>534</v>
@@ -2791,7 +2792,7 @@
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="28"/>
       <c r="B8" s="25">
         <v>70.31</v>
@@ -2806,7 +2807,7 @@
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>13</v>
       </c>
@@ -2823,7 +2824,7 @@
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="28"/>
       <c r="B10" s="25">
         <v>168.21</v>
@@ -2838,7 +2839,7 @@
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>14</v>
       </c>
@@ -2855,7 +2856,7 @@
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="23" t="s">
         <v>23</v>
@@ -2872,7 +2873,7 @@
       <c r="H12" s="23"/>
       <c r="I12" s="23"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>15</v>
       </c>
@@ -2887,7 +2888,7 @@
       <c r="H13" s="26"/>
       <c r="I13" s="26"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>16</v>
       </c>
@@ -2904,7 +2905,7 @@
       <c r="H14" s="26"/>
       <c r="I14" s="26"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="23" t="s">
         <v>23</v>
@@ -2921,7 +2922,7 @@
       <c r="H15" s="23"/>
       <c r="I15" s="23"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>17</v>
       </c>
@@ -2938,7 +2939,7 @@
       <c r="H16" s="23"/>
       <c r="I16" s="23"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>18</v>
       </c>
@@ -2955,7 +2956,7 @@
       <c r="H17" s="23"/>
       <c r="I17" s="23"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>26</v>
       </c>
@@ -2972,7 +2973,7 @@
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>27</v>
       </c>
@@ -2989,7 +2990,7 @@
       <c r="H19" s="26"/>
       <c r="I19" s="26"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="28"/>
       <c r="B20" s="25"/>
       <c r="C20" s="25">
@@ -3019,17 +3020,17 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="91.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="91.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="41"/>
       <c r="C1" s="7"/>
@@ -3039,7 +3040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>60</v>
       </c>
@@ -3051,7 +3052,7 @@
       <c r="E2" s="13"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" s="41"/>
       <c r="C3" s="7"/>
@@ -3059,7 +3060,7 @@
       <c r="E3" s="13"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>62</v>
       </c>
@@ -3079,7 +3080,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D5" s="7" t="s">
         <v>64</v>
       </c>
@@ -3090,7 +3091,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" s="7" t="s">
         <v>65</v>
       </c>
@@ -3099,7 +3100,7 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7" s="7" t="s">
         <v>66</v>
       </c>
@@ -3124,16 +3125,16 @@
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.5" customWidth="1"/>
-    <col min="4" max="4" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.42578125" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>1</v>
       </c>
@@ -3151,7 +3152,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>43586</v>
       </c>
@@ -3166,7 +3167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>43587</v>
       </c>
@@ -3181,7 +3182,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>43588</v>
       </c>
@@ -3196,7 +3197,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
         <v>43617</v>
       </c>
@@ -3221,13 +3222,13 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.1640625" style="38"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -3238,7 +3239,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="30">
         <v>43525</v>
       </c>
@@ -3249,7 +3250,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="30">
         <v>43556</v>
       </c>
@@ -3260,7 +3261,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <v>43586</v>
       </c>

</xml_diff>

<commit_message>
For some reason we're not seeing a previous bug. Trying to force it to happen!
</commit_message>
<xml_diff>
--- a/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
+++ b/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\ManualTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\reconciliation-samples\For-debugging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720D0FA9-E33C-4B1A-BFF5-CE82B40C5CF1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D034CAE4-C692-4BB9-82A8-3BD86169943F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="24735" yWindow="1275" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank In" sheetId="7" r:id="rId1"/>
@@ -1969,7 +1969,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O21" sqref="O21"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2025,6 +2025,7 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
       <c r="L2" s="5">
         <v>43586</v>
       </c>
@@ -2059,6 +2060,7 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
       <c r="L3" s="5">
         <v>43587</v>
       </c>
@@ -2095,6 +2097,7 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
       <c r="L4" s="5">
         <v>43588</v>
       </c>
@@ -2129,6 +2132,7 @@
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
       <c r="L5" s="5">
         <v>43589</v>
       </c>
@@ -2163,6 +2167,7 @@
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
       <c r="L6" s="5">
         <v>43597</v>
       </c>
@@ -2197,6 +2202,7 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
       <c r="L7" s="5">
         <v>43598</v>
       </c>

</xml_diff>

<commit_message>
Recreating changes made in the other branch to get things working in .Net Core (commits 54d3972 to 4c45573 in Refactor-genericise-start)
</commit_message>
<xml_diff>
--- a/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
+++ b/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\reconciliation-samples\For debugging\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\reconciliation-samples\For-debugging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EDA34A-CEDC-43DA-A544-2296E755994D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D034CAE4-C692-4BB9-82A8-3BD86169943F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="24735" yWindow="1275" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank In" sheetId="7" r:id="rId1"/>
@@ -257,7 +257,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="123">
   <si>
     <t>notes</t>
   </si>
@@ -577,9 +577,6 @@
     <t>!! ActualBank bal !!</t>
   </si>
   <si>
-    <t>CRED CARD 2</t>
-  </si>
-  <si>
     <t>"CRED CARD 2"</t>
   </si>
   <si>
@@ -620,6 +617,15 @@
   </si>
   <si>
     <t>CREDIT CARD 2</t>
+  </si>
+  <si>
+    <t>Code042</t>
+  </si>
+  <si>
+    <t>Mortgage description</t>
+  </si>
+  <si>
+    <t>"Mortgage description"</t>
   </si>
 </sst>
 </file>
@@ -1197,7 +1203,7 @@
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" style="9" bestFit="1" customWidth="1"/>
@@ -1374,7 +1380,7 @@
       <selection pane="bottomLeft" activeCell="F2" sqref="F2:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.140625" bestFit="1" customWidth="1"/>
@@ -1419,7 +1425,7 @@
         <v>19</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J2" s="20">
         <v>43616</v>
@@ -1444,7 +1450,7 @@
         <v>20</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J3" s="20"/>
       <c r="K3" s="14">
@@ -1467,7 +1473,7 @@
         <v>19</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K4" s="14">
         <v>3</v>
@@ -1475,7 +1481,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1485,20 +1491,21 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF22F54-1C2B-49C1-90A9-21044AC295B0}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1635,7 +1642,7 @@
         <v>19</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K9" s="20">
         <v>43616</v>
@@ -1649,7 +1656,7 @@
         <v>88</v>
       </c>
       <c r="B10" s="18">
-        <f t="shared" ref="B10:B11" si="0">$K$9+L10</f>
+        <f t="shared" ref="B10:B12" si="0">$K$9+L10</f>
         <v>43618</v>
       </c>
       <c r="C10" s="17">
@@ -1659,7 +1666,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K10" s="20"/>
       <c r="L10" s="14">
@@ -1681,120 +1688,116 @@
         <v>19</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L11" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B12" s="46" t="s">
+    <row r="12" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" s="18">
+        <f t="shared" si="0"/>
+        <v>43620</v>
+      </c>
+      <c r="C12" s="17">
+        <v>1000</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="L12" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B13" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="19"/>
-    </row>
-    <row r="13" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" s="18">
-        <f>$K$9+L13</f>
-        <v>43617</v>
-      </c>
-      <c r="C13" s="17">
-        <v>65</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="L13" s="14">
-        <v>1</v>
-      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="19"/>
     </row>
     <row r="14" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B14" s="18">
-        <f t="shared" ref="B14:B15" si="1">$K$9+L14</f>
-        <v>43618</v>
+        <f>$K$9+L14</f>
+        <v>43617</v>
       </c>
       <c r="C14" s="17">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L14" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="18">
+        <f t="shared" ref="B15:B16" si="1">$K$9+L15</f>
+        <v>43618</v>
+      </c>
+      <c r="C15" s="17">
+        <v>75</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="L15" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B16" s="18">
         <f t="shared" si="1"/>
         <v>43619</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C16" s="17">
         <v>85</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E16" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L16" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="46" t="s">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="B17" s="18">
-        <f>$K$9+L17</f>
-        <v>43617</v>
-      </c>
-      <c r="C17" s="17">
-        <v>95</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="F17" s="14"/>
       <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="14">
-        <v>1</v>
-      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B18" s="18">
-        <f t="shared" ref="B18:B19" si="2">$K$9+L18</f>
-        <v>43618</v>
+        <f>$K$9+L18</f>
+        <v>43617</v>
       </c>
       <c r="C18" s="17">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
@@ -1803,91 +1806,92 @@
       <c r="J18" s="14"/>
       <c r="K18" s="20"/>
       <c r="L18" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" s="18">
-        <f t="shared" si="2"/>
-        <v>43619</v>
+        <f t="shared" ref="B19:B20" si="2">$K$9+L19</f>
+        <v>43618</v>
       </c>
       <c r="C19" s="17">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D19" s="14"/>
       <c r="E19" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
+      <c r="K19" s="20"/>
       <c r="L19" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="18">
+        <f t="shared" si="2"/>
+        <v>43619</v>
+      </c>
+      <c r="C20" s="17">
+        <v>115</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="45" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="12">
-        <f>SUM(C9:C19)</f>
-        <v>675</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
+      <c r="C21" s="12">
+        <f>SUM(C9:C20)</f>
+        <v>1675</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="34" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="18">
-        <v>43466</v>
-      </c>
-      <c r="C23" s="17">
-        <v>125</v>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="14"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" s="18">
-        <v>43647</v>
+        <v>43466</v>
       </c>
       <c r="C24" s="17">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
@@ -1898,34 +1902,58 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B25" s="18">
-        <v>43770</v>
+        <v>43647</v>
       </c>
       <c r="C25" s="17">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
+      <c r="K25" s="20"/>
       <c r="L25" s="14"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="47" t="s">
+      <c r="A26" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="18">
+        <v>43770</v>
+      </c>
+      <c r="C26" s="17">
+        <v>145</v>
+      </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="12">
-        <f>SUM(C23:C25)</f>
+      <c r="C27" s="12">
+        <f>SUM(C24:C26)</f>
         <v>405</v>
       </c>
     </row>
@@ -1937,14 +1965,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C703CDFE-5895-4A70-B218-454B4A08CC66}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2:K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" style="12" bestFit="1" customWidth="1"/>
@@ -1997,6 +2025,7 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
       <c r="L2" s="5">
         <v>43586</v>
       </c>
@@ -2031,6 +2060,7 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
       <c r="L3" s="5">
         <v>43587</v>
       </c>
@@ -2067,6 +2097,7 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
       <c r="L4" s="5">
         <v>43588</v>
       </c>
@@ -2082,7 +2113,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>43597</v>
+        <v>43589</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="29" t="s">
@@ -2091,32 +2122,33 @@
       <c r="D5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>119</v>
+      <c r="E5" s="14" t="s">
+        <v>121</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="13">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
       <c r="L5" s="5">
-        <v>43597</v>
+        <v>43589</v>
       </c>
       <c r="M5">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="N5" t="s">
         <v>46</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>43598</v>
+        <v>43597</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="29" t="s">
@@ -2126,20 +2158,21 @@
         <v>43</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="13">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
       <c r="L6" s="5">
-        <v>43598</v>
+        <v>43597</v>
       </c>
       <c r="M6">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="N6" t="s">
         <v>46</v>
@@ -2149,29 +2182,64 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="5">
+        <v>43598</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="13">
+        <v>1500</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="5">
+        <v>43598</v>
+      </c>
+      <c r="M7">
+        <v>1500</v>
+      </c>
+      <c r="N7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>43616</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B9" s="13">
         <v>5.05</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="7" t="s">
+      <c r="C9" s="13"/>
+      <c r="D9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E9" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2185,10 +2253,10 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="38" bestFit="1" customWidth="1"/>
@@ -2196,7 +2264,7 @@
     <col min="4" max="4" width="30.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2322,7 +2390,7 @@
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="38" bestFit="1" customWidth="1"/>
@@ -2330,7 +2398,7 @@
     <col min="4" max="4" width="30.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2453,10 +2521,10 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:A8"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" style="38" bestFit="1" customWidth="1"/>
@@ -2608,11 +2676,11 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD28"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -2958,11 +3026,11 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="91.140625" bestFit="1" customWidth="1"/>
@@ -3015,7 +3083,7 @@
         <v>-1000</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3026,7 +3094,7 @@
         <v>-1000</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3046,7 +3114,7 @@
         <v>-1000</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -3063,7 +3131,7 @@
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" style="38" bestFit="1" customWidth="1"/>
@@ -3160,7 +3228,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.140625" style="38"/>

</xml_diff>

<commit_message>
Update test data to current year.
</commit_message>
<xml_diff>
--- a/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
+++ b/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\reconciliation-samples\For-debugging\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\Reconciliate\reconciliation-samples\For-debugging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D034CAE4-C692-4BB9-82A8-3BD86169943F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0806303B-20CF-4CA7-ABBA-C96F5137683D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24735" yWindow="1275" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="825" yWindow="105" windowWidth="22905" windowHeight="12285" firstSheet="3" activeTab="10" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank In" sheetId="7" r:id="rId1"/>
@@ -249,7 +249,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1200,7 +1202,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,7 +1239,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>43586</v>
+        <v>43952</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="29" t="s">
@@ -1257,7 +1259,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="L2" s="5">
-        <v>43586</v>
+        <v>43952</v>
       </c>
       <c r="M2">
         <v>5</v>
@@ -1271,7 +1273,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>43587</v>
+        <v>43953</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="29" t="s">
@@ -1291,7 +1293,7 @@
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="L3" s="5">
-        <v>43587</v>
+        <v>43953</v>
       </c>
       <c r="M3">
         <v>10</v>
@@ -1305,7 +1307,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>43588</v>
+        <v>43954</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="29" t="s">
@@ -1327,7 +1329,7 @@
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="L4" s="5">
-        <v>43588</v>
+        <v>43954</v>
       </c>
       <c r="M4">
         <v>15</v>
@@ -1347,7 +1349,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>43616</v>
+        <v>43982</v>
       </c>
       <c r="B6" s="13">
         <v>5.05</v>
@@ -1493,7 +1495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF22F54-1C2B-49C1-90A9-21044AC295B0}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
@@ -1967,9 +1969,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C703CDFE-5895-4A70-B218-454B4A08CC66}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2:K7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2006,7 +2008,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>43586</v>
+        <v>43952</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="29" t="s">
@@ -2027,7 +2029,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="5">
-        <v>43586</v>
+        <v>43952</v>
       </c>
       <c r="M2">
         <v>5</v>
@@ -2041,7 +2043,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>43587</v>
+        <v>43953</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="29" t="s">
@@ -2062,7 +2064,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
       <c r="L3" s="5">
-        <v>43587</v>
+        <v>43953</v>
       </c>
       <c r="M3">
         <v>10</v>
@@ -2076,7 +2078,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>43588</v>
+        <v>43954</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="29" t="s">
@@ -2099,7 +2101,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="5">
-        <v>43588</v>
+        <v>43954</v>
       </c>
       <c r="M4">
         <v>15</v>
@@ -2113,7 +2115,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>43589</v>
+        <v>43955</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="29" t="s">
@@ -2134,7 +2136,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="5">
-        <v>43589</v>
+        <v>43955</v>
       </c>
       <c r="M5">
         <v>1000</v>
@@ -2148,7 +2150,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>43597</v>
+        <v>43963</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="29" t="s">
@@ -2169,7 +2171,7 @@
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="5">
-        <v>43597</v>
+        <v>43963</v>
       </c>
       <c r="M6">
         <v>500</v>
@@ -2183,7 +2185,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>43598</v>
+        <v>43964</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="29" t="s">
@@ -2204,7 +2206,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="5">
-        <v>43598</v>
+        <v>43964</v>
       </c>
       <c r="M7">
         <v>1500</v>
@@ -2223,7 +2225,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>43616</v>
+        <v>43982</v>
       </c>
       <c r="B9" s="13">
         <v>5.05</v>
@@ -2253,7 +2255,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2287,7 +2289,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>43586</v>
+        <v>43952</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="29" t="s">
@@ -2300,7 +2302,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="5">
-        <v>43586</v>
+        <v>43952</v>
       </c>
       <c r="I2">
         <v>5</v>
@@ -2311,7 +2313,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>43587</v>
+        <v>43953</v>
       </c>
       <c r="B3" s="37"/>
       <c r="C3" s="29" t="s">
@@ -2324,7 +2326,7 @@
         <v>10</v>
       </c>
       <c r="H3" s="5">
-        <v>43587</v>
+        <v>43953</v>
       </c>
       <c r="I3">
         <v>10</v>
@@ -2335,7 +2337,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>43588</v>
+        <v>43954</v>
       </c>
       <c r="B4" s="37"/>
       <c r="C4" s="29" t="s">
@@ -2348,7 +2350,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="5">
-        <v>43588</v>
+        <v>43954</v>
       </c>
       <c r="I4">
         <v>15</v>
@@ -2365,7 +2367,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>43616</v>
+        <v>43982</v>
       </c>
       <c r="B6" s="37">
         <v>10</v>
@@ -2387,7 +2389,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2421,7 +2423,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>43586</v>
+        <v>43952</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="29" t="s">
@@ -2434,7 +2436,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="5">
-        <v>43586</v>
+        <v>43952</v>
       </c>
       <c r="I2">
         <v>5</v>
@@ -2445,7 +2447,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>43587</v>
+        <v>43953</v>
       </c>
       <c r="B3" s="37"/>
       <c r="C3" s="29" t="s">
@@ -2458,7 +2460,7 @@
         <v>10</v>
       </c>
       <c r="H3" s="5">
-        <v>43587</v>
+        <v>43953</v>
       </c>
       <c r="I3">
         <v>10</v>
@@ -2469,7 +2471,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>43588</v>
+        <v>43954</v>
       </c>
       <c r="B4" s="37"/>
       <c r="C4" s="29" t="s">
@@ -2482,7 +2484,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="5">
-        <v>43588</v>
+        <v>43954</v>
       </c>
       <c r="I4">
         <v>15</v>
@@ -2499,7 +2501,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>43616</v>
+        <v>43982</v>
       </c>
       <c r="B6" s="37">
         <v>10</v>
@@ -2521,7 +2523,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,7 +2566,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>43586</v>
+        <v>43952</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>11</v>
@@ -2573,7 +2575,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="5">
-        <v>43586</v>
+        <v>43952</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>49</v>
@@ -2581,7 +2583,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>43587</v>
+        <v>43953</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>11</v>
@@ -2590,7 +2592,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="5">
-        <v>43587</v>
+        <v>43953</v>
       </c>
       <c r="F3" s="38">
         <v>25</v>
@@ -2601,7 +2603,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>43588</v>
+        <v>43954</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>12</v>
@@ -2610,7 +2612,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="5">
-        <v>43588</v>
+        <v>43954</v>
       </c>
       <c r="F4" s="38">
         <v>25</v>
@@ -2626,7 +2628,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>43617</v>
+        <v>43983</v>
       </c>
       <c r="B6" s="38">
         <v>20</v>
@@ -2640,7 +2642,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>43618</v>
+        <v>43984</v>
       </c>
       <c r="B7" s="38">
         <v>25</v>
@@ -2654,7 +2656,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>43619</v>
+        <v>43985</v>
       </c>
       <c r="B8" s="38">
         <v>30</v>
@@ -3128,7 +3130,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3160,7 +3162,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>43586</v>
+        <v>43952</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="29" t="s">
@@ -3175,7 +3177,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>43587</v>
+        <v>43953</v>
       </c>
       <c r="B3" s="37"/>
       <c r="C3" s="29" t="s">
@@ -3190,7 +3192,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>43588</v>
+        <v>43954</v>
       </c>
       <c r="B4" s="37"/>
       <c r="C4" s="29" t="s">
@@ -3205,7 +3207,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
-        <v>43617</v>
+        <v>43983</v>
       </c>
       <c r="B5" s="38">
         <v>20</v>
@@ -3247,7 +3249,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="30">
-        <v>43525</v>
+        <v>43891</v>
       </c>
       <c r="B2" s="38">
         <v>100</v>
@@ -3258,7 +3260,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="30">
-        <v>43556</v>
+        <v>43922</v>
       </c>
       <c r="B3" s="38">
         <v>100</v>
@@ -3269,7 +3271,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
-        <v>43586</v>
+        <v>43952</v>
       </c>
       <c r="B4" s="38">
         <v>100</v>

</xml_diff>

<commit_message>
Change test data dates to current date.
</commit_message>
<xml_diff>
--- a/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
+++ b/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\Reconciliate\reconciliation-samples\For-debugging\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\reconciliation-samples\For-debugging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0806303B-20CF-4CA7-ABBA-C96F5137683D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833B64D4-5DB8-46B2-BECA-D647E0612CB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="825" yWindow="105" windowWidth="22905" windowHeight="12285" firstSheet="3" activeTab="10" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
@@ -609,9 +609,6 @@
     <t>!! CredCard2 bal recorded from statement dated April 2019</t>
   </si>
   <si>
-    <t>!! CredCard1 bal recorded from statement dated April 2019</t>
-  </si>
-  <si>
     <t>!! &lt;-- leftmost column - ActualBank bal recorded from downloaded csv, row "30/4/19, £100, Some Description"</t>
   </si>
   <si>
@@ -628,14 +625,16 @@
   </si>
   <si>
     <t>"Mortgage description"</t>
+  </si>
+  <si>
+    <t>!! CredCard1 bal recorded from statement dated May 2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0.00"/>
@@ -760,17 +759,17 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1"/>
@@ -1698,7 +1697,7 @@
     </row>
     <row r="12" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B12" s="18">
         <f t="shared" si="0"/>
@@ -1711,7 +1710,7 @@
         <v>19</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L12" s="14">
         <v>4</v>
@@ -2125,7 +2124,7 @@
         <v>43</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="13">
@@ -2145,7 +2144,7 @@
         <v>46</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2160,7 +2159,7 @@
         <v>43</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="13">
@@ -2195,7 +2194,7 @@
         <v>43</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="13">
@@ -3085,7 +3084,7 @@
         <v>-1000</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3096,7 +3095,7 @@
         <v>-1000</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Data updated by running tests.
</commit_message>
<xml_diff>
--- a/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
+++ b/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\reconciliation-samples\For-debugging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833B64D4-5DB8-46B2-BECA-D647E0612CB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC3E768-4E9A-48DE-A280-EFB7FB969A93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="825" yWindow="105" windowWidth="22905" windowHeight="12285" firstSheet="3" activeTab="10" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
@@ -259,7 +259,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="166">
   <si>
     <t>notes</t>
   </si>
@@ -606,9 +606,6 @@
     <t>Bank monthly outgoing transaction 03</t>
   </si>
   <si>
-    <t>!! CredCard2 bal recorded from statement dated April 2019</t>
-  </si>
-  <si>
     <t>!! &lt;-- leftmost column - ActualBank bal recorded from downloaded csv, row "30/4/19, £100, Some Description"</t>
   </si>
   <si>
@@ -628,6 +625,138 @@
   </si>
   <si>
     <t>!! CredCard1 bal recorded from statement dated May 2020</t>
+  </si>
+  <si>
+    <t>"CredCard1 monthly transaction 01"</t>
+  </si>
+  <si>
+    <t>"Greens"</t>
+  </si>
+  <si>
+    <t>"CredCard1 monthly transaction 02"</t>
+  </si>
+  <si>
+    <t>"CredCard1 monthly transaction 03"</t>
+  </si>
+  <si>
+    <t>!! Unmatched from 3rd party: "Jam Kippers"</t>
+  </si>
+  <si>
+    <t>"Jam Kippers"</t>
+  </si>
+  <si>
+    <t>!! Unmatched from 3rd party: "CredCard1 transaction from CredCard1.csv"</t>
+  </si>
+  <si>
+    <t>"CredCard1 transaction from CredCard1.csv"</t>
+  </si>
+  <si>
+    <t>"CRED CARD 1 PAYMENT DESCRIPTION ON STATEMENTS"</t>
+  </si>
+  <si>
+    <t>Divider</t>
+  </si>
+  <si>
+    <t>"left over from previous reconciliation"</t>
+  </si>
+  <si>
+    <t>"CredCard1 transaction from CredCard1InOutPending.csv"</t>
+  </si>
+  <si>
+    <t>"Halloumi Icecream"</t>
+  </si>
+  <si>
+    <t>!! CredCard2 bal recorded from statement dated May 2020</t>
+  </si>
+  <si>
+    <t>"CredCard2 monthly transaction 01"</t>
+  </si>
+  <si>
+    <t>"Eglantine"</t>
+  </si>
+  <si>
+    <t>"EGLANTINE"</t>
+  </si>
+  <si>
+    <t>"CredCard2 monthly transaction 02"</t>
+  </si>
+  <si>
+    <t>"Fennel"</t>
+  </si>
+  <si>
+    <t>"FENNEL"</t>
+  </si>
+  <si>
+    <t>"CredCard2 monthly transaction 03"</t>
+  </si>
+  <si>
+    <t>!! Unmatched from 3rd party: "CredCard2 transaction from CredCard2.csv"</t>
+  </si>
+  <si>
+    <t>"CredCard2 transaction from CredCard2.csv"</t>
+  </si>
+  <si>
+    <t>"CRED CARD 2 PAYMENT DESCRIPTION ON STATEMENTS"</t>
+  </si>
+  <si>
+    <t>"CredCard2 transaction from pending.txt"</t>
+  </si>
+  <si>
+    <t>"Bank monthly incoming transaction 01"</t>
+  </si>
+  <si>
+    <t>"'Bank monthly incoming transaction 01"</t>
+  </si>
+  <si>
+    <t>"Bank monthly incoming transaction 02"</t>
+  </si>
+  <si>
+    <t>"'Bank monthly incoming transaction 02"</t>
+  </si>
+  <si>
+    <t>"Bank monthly incoming transaction 03"</t>
+  </si>
+  <si>
+    <t>"'Bank monthly incoming transaction 03"</t>
+  </si>
+  <si>
+    <t>Type2</t>
+  </si>
+  <si>
+    <t>"Cheese "</t>
+  </si>
+  <si>
+    <t>"'Cheese"</t>
+  </si>
+  <si>
+    <t>Type3</t>
+  </si>
+  <si>
+    <t>"Doughnut Platypus"</t>
+  </si>
+  <si>
+    <t>"'Doughnut Pumpernickel"</t>
+  </si>
+  <si>
+    <t>!! Unmatched from 3rd party: "'BankIn transaction from ActualBank.csv"</t>
+  </si>
+  <si>
+    <t>"'BankIn transaction from ActualBank.csv"</t>
+  </si>
+  <si>
+    <t>"first expense"</t>
+  </si>
+  <si>
+    <t>"second expense"</t>
+  </si>
+  <si>
+    <t>Type1</t>
+  </si>
+  <si>
+    <t>"BankIn transaction from pending.txt"</t>
+  </si>
+  <si>
+    <t>"third expense"</t>
   </si>
 </sst>
 </file>
@@ -763,9 +892,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -783,6 +909,7 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1197,7 +1324,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B106CA6-6EF5-459F-BBFA-85FA2D21E2D2}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1347,24 +1474,253 @@
       <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="1">
+        <v>43983</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="9">
+        <v>21.76</v>
+      </c>
+      <c r="L6" s="30">
+        <v>43983</v>
+      </c>
+      <c r="M6">
+        <v>21.76</v>
+      </c>
+      <c r="N6" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43984</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G7" s="9">
+        <v>15.6</v>
+      </c>
+      <c r="L7" s="30">
+        <v>43984</v>
+      </c>
+      <c r="M7">
+        <v>15.6</v>
+      </c>
+      <c r="N7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43985</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>151</v>
+      </c>
+      <c r="G8" s="9">
+        <v>54.97</v>
+      </c>
+      <c r="L8" s="30">
+        <v>43985</v>
+      </c>
+      <c r="M8">
+        <v>54.97</v>
+      </c>
+      <c r="N8" t="s">
+        <v>46</v>
+      </c>
+      <c r="O8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43992</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" t="s">
+        <v>154</v>
+      </c>
+      <c r="G9" s="9">
+        <v>222</v>
+      </c>
+      <c r="L9" s="30">
+        <v>43992</v>
+      </c>
+      <c r="M9">
+        <v>222</v>
+      </c>
+      <c r="N9" t="s">
+        <v>46</v>
+      </c>
+      <c r="O9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43993</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>156</v>
+      </c>
+      <c r="E10" t="s">
+        <v>157</v>
+      </c>
+      <c r="G10" s="9">
+        <v>333</v>
+      </c>
+      <c r="L10" s="30">
+        <v>43993</v>
+      </c>
+      <c r="M10">
+        <v>333</v>
+      </c>
+      <c r="N10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43993</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>159</v>
+      </c>
+      <c r="G11" s="9">
+        <v>444</v>
+      </c>
+      <c r="L11" s="30">
+        <v>43993</v>
+      </c>
+      <c r="M11">
+        <v>444</v>
+      </c>
+      <c r="N11" t="s">
+        <v>46</v>
+      </c>
+      <c r="O11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>43982</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B13" s="9">
         <v>5.05</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="7" t="s">
+      <c r="D13" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="E13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B14" s="9">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43984</v>
+      </c>
+      <c r="B15" s="9">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>43985</v>
+      </c>
+      <c r="B16" s="9">
+        <v>111</v>
+      </c>
+      <c r="D16" t="s">
+        <v>163</v>
+      </c>
+      <c r="E16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>43985</v>
+      </c>
+      <c r="B17" s="9">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" t="s">
+        <v>165</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1390,7 +1746,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="44" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="34" t="s">
@@ -1481,7 +1837,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="48" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1604,7 +1960,7 @@
       <c r="B6" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="48">
+      <c r="C6" s="47">
         <f>SUM(C3:C5)</f>
         <v>45</v>
       </c>
@@ -1697,7 +2053,7 @@
     </row>
     <row r="12" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B12" s="18">
         <f t="shared" si="0"/>
@@ -1710,14 +2066,14 @@
         <v>19</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L12" s="14">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="45" t="s">
         <v>75</v>
       </c>
       <c r="C13" s="18"/>
@@ -1780,7 +2136,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="45" t="s">
         <v>76</v>
       </c>
       <c r="G17" s="14"/>
@@ -1861,7 +2217,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="44" t="s">
         <v>77</v>
       </c>
       <c r="C21" s="12">
@@ -1950,7 +2306,7 @@
       <c r="L26" s="14"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="47" t="s">
+      <c r="B27" s="46" t="s">
         <v>79</v>
       </c>
       <c r="C27" s="12">
@@ -2124,7 +2480,7 @@
         <v>43</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="13">
@@ -2144,7 +2500,7 @@
         <v>46</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2159,7 +2515,7 @@
         <v>43</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="13">
@@ -2194,7 +2550,7 @@
         <v>43</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="13">
@@ -2250,7 +2606,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D874970E-DFC7-41AF-9C75-179A4BAE8469}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2365,16 +2721,203 @@
       <c r="D5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="1">
+        <v>43983</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6">
+        <v>65</v>
+      </c>
+      <c r="H6" s="30">
+        <v>43983</v>
+      </c>
+      <c r="I6">
+        <v>65</v>
+      </c>
+      <c r="J6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43984</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7">
+        <v>22</v>
+      </c>
+      <c r="H7" s="30">
+        <v>43984</v>
+      </c>
+      <c r="I7">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43984</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8">
+        <v>75</v>
+      </c>
+      <c r="H8" s="30">
+        <v>43984</v>
+      </c>
+      <c r="I8">
+        <v>75</v>
+      </c>
+      <c r="J8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43985</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9">
+        <v>85</v>
+      </c>
+      <c r="H9" s="30">
+        <v>43985</v>
+      </c>
+      <c r="I9">
+        <v>85</v>
+      </c>
+      <c r="J9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43985</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10">
+        <v>33</v>
+      </c>
+      <c r="H10" s="30">
+        <v>43985</v>
+      </c>
+      <c r="I10">
+        <v>33</v>
+      </c>
+      <c r="J10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43986</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11">
+        <v>44</v>
+      </c>
+      <c r="H11" s="30">
+        <v>43986</v>
+      </c>
+      <c r="I11">
+        <v>44</v>
+      </c>
+      <c r="J11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43994</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="E12">
+        <v>-1000</v>
+      </c>
+      <c r="H12" s="30">
+        <v>43994</v>
+      </c>
+      <c r="I12">
+        <v>-1000</v>
+      </c>
+      <c r="J12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="38" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>43982</v>
       </c>
-      <c r="B6" s="37">
+      <c r="B14" s="38">
         <v>10</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="13"/>
+      <c r="D14" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B15" s="38">
+        <v>11</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>43985</v>
+      </c>
+      <c r="B16" s="38">
+        <v>33</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>134</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2384,7 +2927,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A79CC3C-10DD-4C9D-955D-781259440CED}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2499,16 +3042,192 @@
       <c r="D5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="1">
+        <v>43983</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6">
+        <v>95</v>
+      </c>
+      <c r="H6" s="30">
+        <v>43983</v>
+      </c>
+      <c r="I6">
+        <v>95</v>
+      </c>
+      <c r="J6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43984</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E7">
+        <v>66</v>
+      </c>
+      <c r="H7" s="30">
+        <v>43984</v>
+      </c>
+      <c r="I7">
+        <v>66</v>
+      </c>
+      <c r="J7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43984</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8">
+        <v>105</v>
+      </c>
+      <c r="H8" s="30">
+        <v>43984</v>
+      </c>
+      <c r="I8">
+        <v>105</v>
+      </c>
+      <c r="J8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43985</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E9">
+        <v>77</v>
+      </c>
+      <c r="H9" s="30">
+        <v>43986</v>
+      </c>
+      <c r="I9">
+        <v>77</v>
+      </c>
+      <c r="J9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43985</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10">
+        <v>115</v>
+      </c>
+      <c r="H10" s="30">
+        <v>43985</v>
+      </c>
+      <c r="I10">
+        <v>115</v>
+      </c>
+      <c r="J10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43987</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E11">
+        <v>88</v>
+      </c>
+      <c r="H11" s="30">
+        <v>43987</v>
+      </c>
+      <c r="I11">
+        <v>88</v>
+      </c>
+      <c r="J11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43995</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="E12">
+        <v>-2000</v>
+      </c>
+      <c r="H12" s="30">
+        <v>43995</v>
+      </c>
+      <c r="I12">
+        <v>-2000</v>
+      </c>
+      <c r="J12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="38" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>43982</v>
       </c>
-      <c r="B6" s="37">
+      <c r="B14" s="38">
         <v>10</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="13"/>
+      <c r="D14" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B15" s="38">
+        <v>55</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>146</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2626,44 +3345,53 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="30">
         <v>43983</v>
       </c>
       <c r="B6" s="38">
         <v>20</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="E6" s="49">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="30">
         <v>43984</v>
       </c>
       <c r="B7" s="38">
         <v>25</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="E7" s="49">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="30">
         <v>43985</v>
       </c>
       <c r="B8" s="38">
         <v>30</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="E8" s="49">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
         <v>59</v>
       </c>
     </row>
@@ -3039,7 +3767,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="41"/>
+      <c r="B1" s="40"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="13"/>
@@ -3051,7 +3779,7 @@
       <c r="A2" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="41"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="7"/>
       <c r="D2" s="34" t="s">
         <v>61</v>
@@ -3061,7 +3789,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
-      <c r="B3" s="41"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="7"/>
       <c r="D3" s="34"/>
       <c r="E3" s="13"/>
@@ -3071,10 +3799,10 @@
       <c r="A4" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="41">
+      <c r="B4" s="40">
         <v>1000</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="41" t="s">
         <v>105</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -3084,7 +3812,7 @@
         <v>-1000</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3095,7 +3823,7 @@
         <v>-1000</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3112,10 +3840,10 @@
         <v>66</v>
       </c>
       <c r="E7" s="13">
-        <v>-1000</v>
+        <v>-2000</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -3152,7 +3880,7 @@
       <c r="D1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="43" t="s">
         <v>68</v>
       </c>
       <c r="F1" s="34" t="s">
@@ -3239,10 +3967,10 @@
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="42" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New test data for budgeting monthly dates
</commit_message>
<xml_diff>
--- a/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
+++ b/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\reconciliation-samples\For-debugging\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\Reconciliate\reconciliation-samples\For-debugging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC3E768-4E9A-48DE-A280-EFB7FB969A93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDE57F7-67E9-480F-853B-0D25BD636C10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="105" windowWidth="22905" windowHeight="12285" firstSheet="3" activeTab="10" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="24090" yWindow="630" windowWidth="18525" windowHeight="12285" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank In" sheetId="7" r:id="rId1"/>
@@ -259,7 +259,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="127">
   <si>
     <t>notes</t>
   </si>
@@ -588,9 +588,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Bank monthly incoming transaction 01</t>
-  </si>
-  <si>
     <t>Bank monthly incoming transaction 02</t>
   </si>
   <si>
@@ -621,149 +618,36 @@
     <t>Mortgage description</t>
   </si>
   <si>
-    <t>"Mortgage description"</t>
-  </si>
-  <si>
     <t>!! CredCard1 bal recorded from statement dated May 2020</t>
   </si>
   <si>
-    <t>"CredCard1 monthly transaction 01"</t>
-  </si>
-  <si>
-    <t>"Greens"</t>
-  </si>
-  <si>
-    <t>"CredCard1 monthly transaction 02"</t>
-  </si>
-  <si>
-    <t>"CredCard1 monthly transaction 03"</t>
-  </si>
-  <si>
-    <t>!! Unmatched from 3rd party: "Jam Kippers"</t>
-  </si>
-  <si>
-    <t>"Jam Kippers"</t>
-  </si>
-  <si>
-    <t>!! Unmatched from 3rd party: "CredCard1 transaction from CredCard1.csv"</t>
-  </si>
-  <si>
-    <t>"CredCard1 transaction from CredCard1.csv"</t>
-  </si>
-  <si>
-    <t>"CRED CARD 1 PAYMENT DESCRIPTION ON STATEMENTS"</t>
-  </si>
-  <si>
     <t>Divider</t>
   </si>
   <si>
-    <t>"left over from previous reconciliation"</t>
-  </si>
-  <si>
-    <t>"CredCard1 transaction from CredCard1InOutPending.csv"</t>
-  </si>
-  <si>
-    <t>"Halloumi Icecream"</t>
-  </si>
-  <si>
     <t>!! CredCard2 bal recorded from statement dated May 2020</t>
   </si>
   <si>
-    <t>"CredCard2 monthly transaction 01"</t>
-  </si>
-  <si>
-    <t>"Eglantine"</t>
-  </si>
-  <si>
-    <t>"EGLANTINE"</t>
-  </si>
-  <si>
-    <t>"CredCard2 monthly transaction 02"</t>
-  </si>
-  <si>
-    <t>"Fennel"</t>
-  </si>
-  <si>
-    <t>"FENNEL"</t>
-  </si>
-  <si>
-    <t>"CredCard2 monthly transaction 03"</t>
-  </si>
-  <si>
-    <t>!! Unmatched from 3rd party: "CredCard2 transaction from CredCard2.csv"</t>
-  </si>
-  <si>
-    <t>"CredCard2 transaction from CredCard2.csv"</t>
-  </si>
-  <si>
-    <t>"CRED CARD 2 PAYMENT DESCRIPTION ON STATEMENTS"</t>
-  </si>
-  <si>
-    <t>"CredCard2 transaction from pending.txt"</t>
-  </si>
-  <si>
-    <t>"Bank monthly incoming transaction 01"</t>
-  </si>
-  <si>
-    <t>"'Bank monthly incoming transaction 01"</t>
-  </si>
-  <si>
-    <t>"Bank monthly incoming transaction 02"</t>
-  </si>
-  <si>
-    <t>"'Bank monthly incoming transaction 02"</t>
-  </si>
-  <si>
-    <t>"Bank monthly incoming transaction 03"</t>
-  </si>
-  <si>
-    <t>"'Bank monthly incoming transaction 03"</t>
-  </si>
-  <si>
-    <t>Type2</t>
-  </si>
-  <si>
-    <t>"Cheese "</t>
-  </si>
-  <si>
-    <t>"'Cheese"</t>
-  </si>
-  <si>
-    <t>Type3</t>
-  </si>
-  <si>
-    <t>"Doughnut Platypus"</t>
-  </si>
-  <si>
-    <t>"'Doughnut Pumpernickel"</t>
-  </si>
-  <si>
-    <t>!! Unmatched from 3rd party: "'BankIn transaction from ActualBank.csv"</t>
-  </si>
-  <si>
-    <t>"'BankIn transaction from ActualBank.csv"</t>
-  </si>
-  <si>
-    <t>"first expense"</t>
-  </si>
-  <si>
-    <t>"second expense"</t>
-  </si>
-  <si>
-    <t>Type1</t>
-  </si>
-  <si>
-    <t>"BankIn transaction from pending.txt"</t>
-  </si>
-  <si>
-    <t>"third expense"</t>
+    <t>ACME LTD</t>
+  </si>
+  <si>
+    <t>"'ACME LTD"</t>
+  </si>
+  <si>
+    <t>"Bank monthly outgoing transaction 01"</t>
+  </si>
+  <si>
+    <t>MBNA monthly transaction 01</t>
+  </si>
+  <si>
+    <t>AmEx monthly transaction 01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0.00"/>
@@ -835,7 +719,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -910,6 +794,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1324,11 +1210,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B106CA6-6EF5-459F-BBFA-85FA2D21E2D2}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2:L4"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,9 +1251,9 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>43952</v>
-      </c>
-      <c r="B2" s="13"/>
+        <v>43922</v>
+      </c>
+      <c r="B2" s="37"/>
       <c r="C2" s="29" t="s">
         <v>44</v>
       </c>
@@ -1375,31 +1261,31 @@
         <v>43</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>49</v>
+        <v>122</v>
       </c>
       <c r="F2" s="10"/>
-      <c r="G2" s="13">
-        <v>5</v>
+      <c r="G2" s="37">
+        <v>1000</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="L2" s="5">
-        <v>43952</v>
+        <v>43922</v>
       </c>
       <c r="M2">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="N2" t="s">
         <v>46</v>
       </c>
       <c r="O2" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>43953</v>
+        <v>43952</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="29" t="s">
@@ -1413,16 +1299,16 @@
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="L3" s="5">
-        <v>43953</v>
+        <v>43952</v>
       </c>
       <c r="M3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N3" t="s">
         <v>46</v>
@@ -1433,9 +1319,9 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>43954</v>
-      </c>
-      <c r="B4" s="6"/>
+        <v>43953</v>
+      </c>
+      <c r="B4" s="13"/>
       <c r="C4" s="29" t="s">
         <v>44</v>
       </c>
@@ -1445,20 +1331,18 @@
       <c r="E4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="10">
-        <v>12345</v>
-      </c>
-      <c r="G4" s="6">
-        <v>15</v>
+      <c r="F4" s="10"/>
+      <c r="G4" s="13">
+        <v>10</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="L4" s="5">
-        <v>43954</v>
+        <v>43953</v>
       </c>
       <c r="M4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N4" t="s">
         <v>46</v>
@@ -1468,258 +1352,58 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="12"/>
+      <c r="A5" s="5">
+        <v>43954</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="10">
+        <v>12345</v>
+      </c>
+      <c r="G5" s="6">
+        <v>15</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="L5" s="5">
+        <v>43954</v>
+      </c>
+      <c r="M5">
+        <v>15</v>
+      </c>
+      <c r="N5" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>43983</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>147</v>
-      </c>
-      <c r="G6" s="9">
-        <v>21.76</v>
-      </c>
-      <c r="L6" s="30">
-        <v>43983</v>
-      </c>
-      <c r="M6">
-        <v>21.76</v>
-      </c>
-      <c r="N6" t="s">
-        <v>46</v>
-      </c>
-      <c r="O6" t="s">
-        <v>148</v>
+      <c r="B6" s="9" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>43984</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
+        <v>43982</v>
+      </c>
+      <c r="B7" s="9">
+        <v>5.05</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>149</v>
-      </c>
-      <c r="G7" s="9">
-        <v>15.6</v>
-      </c>
-      <c r="L7" s="30">
-        <v>43984</v>
-      </c>
-      <c r="M7">
-        <v>15.6</v>
-      </c>
-      <c r="N7" t="s">
-        <v>46</v>
-      </c>
-      <c r="O7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>43985</v>
-      </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>151</v>
-      </c>
-      <c r="G8" s="9">
-        <v>54.97</v>
-      </c>
-      <c r="L8" s="30">
-        <v>43985</v>
-      </c>
-      <c r="M8">
-        <v>54.97</v>
-      </c>
-      <c r="N8" t="s">
-        <v>46</v>
-      </c>
-      <c r="O8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>43992</v>
-      </c>
-      <c r="C9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" t="s">
-        <v>153</v>
-      </c>
-      <c r="E9" t="s">
-        <v>154</v>
-      </c>
-      <c r="G9" s="9">
-        <v>222</v>
-      </c>
-      <c r="L9" s="30">
-        <v>43992</v>
-      </c>
-      <c r="M9">
-        <v>222</v>
-      </c>
-      <c r="N9" t="s">
-        <v>46</v>
-      </c>
-      <c r="O9" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>43993</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" t="s">
-        <v>156</v>
-      </c>
-      <c r="E10" t="s">
-        <v>157</v>
-      </c>
-      <c r="G10" s="9">
-        <v>333</v>
-      </c>
-      <c r="L10" s="30">
-        <v>43993</v>
-      </c>
-      <c r="M10">
-        <v>333</v>
-      </c>
-      <c r="N10" t="s">
-        <v>46</v>
-      </c>
-      <c r="O10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>43993</v>
-      </c>
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" t="s">
-        <v>159</v>
-      </c>
-      <c r="G11" s="9">
-        <v>444</v>
-      </c>
-      <c r="L11" s="30">
-        <v>43993</v>
-      </c>
-      <c r="M11">
-        <v>444</v>
-      </c>
-      <c r="N11" t="s">
-        <v>46</v>
-      </c>
-      <c r="O11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>43982</v>
-      </c>
-      <c r="B13" s="9">
-        <v>5.05</v>
-      </c>
-      <c r="D13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>43983</v>
-      </c>
-      <c r="B14" s="9">
-        <v>20</v>
-      </c>
-      <c r="D14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>43984</v>
-      </c>
-      <c r="B15" s="9">
-        <v>25</v>
-      </c>
-      <c r="D15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>43985</v>
-      </c>
-      <c r="B16" s="9">
-        <v>111</v>
-      </c>
-      <c r="D16" t="s">
-        <v>163</v>
-      </c>
-      <c r="E16" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>43985</v>
-      </c>
-      <c r="B17" s="9">
-        <v>30</v>
-      </c>
-      <c r="D17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" t="s">
-        <v>165</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1734,12 +1418,13 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F4"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
@@ -1775,14 +1460,14 @@
         <v>43617</v>
       </c>
       <c r="C2" s="17">
-        <v>21.762</v>
+        <v>1000</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="J2" s="20">
         <v>43616</v>
@@ -1807,7 +1492,7 @@
         <v>20</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J3" s="20"/>
       <c r="K3" s="14">
@@ -1830,7 +1515,7 @@
         <v>19</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K4" s="14">
         <v>3</v>
@@ -1850,7 +1535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF22F54-1C2B-49C1-90A9-21044AC295B0}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
@@ -1999,7 +1684,7 @@
         <v>19</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K9" s="20">
         <v>43616</v>
@@ -2023,7 +1708,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K10" s="20"/>
       <c r="L10" s="14">
@@ -2045,7 +1730,7 @@
         <v>19</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L11" s="14">
         <v>3</v>
@@ -2053,7 +1738,7 @@
     </row>
     <row r="12" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" s="18">
         <f t="shared" si="0"/>
@@ -2066,7 +1751,7 @@
         <v>19</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L12" s="14">
         <v>4</v>
@@ -2326,7 +2011,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A9"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2480,11 +2165,11 @@
         <v>43</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="13">
-        <v>1000</v>
+        <v>35</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -2494,13 +2179,13 @@
         <v>43955</v>
       </c>
       <c r="M5">
-        <v>1000</v>
+        <v>35</v>
       </c>
       <c r="N5" t="s">
         <v>46</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2515,7 +2200,7 @@
         <v>43</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="13">
@@ -2550,7 +2235,7 @@
         <v>43</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="13">
@@ -2606,16 +2291,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D874970E-DFC7-41AF-9C75-179A4BAE8469}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2:H4"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2.140625" customWidth="1"/>
     <col min="4" max="4" width="30.85546875" style="12" bestFit="1" customWidth="1"/>
@@ -2715,208 +2400,43 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5"/>
+      <c r="A5" s="5">
+        <v>43985</v>
+      </c>
+      <c r="B5" s="37"/>
+      <c r="C5" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="50">
+        <v>65</v>
+      </c>
+      <c r="H5" s="5">
+        <v>43985</v>
+      </c>
+      <c r="I5">
+        <v>65</v>
+      </c>
+      <c r="J5" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>43983</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6">
-        <v>65</v>
-      </c>
-      <c r="H6" s="30">
-        <v>43983</v>
-      </c>
-      <c r="I6">
-        <v>65</v>
-      </c>
-      <c r="J6" t="s">
-        <v>122</v>
+      <c r="B6" s="38" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>43984</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
+        <v>43982</v>
+      </c>
+      <c r="B7" s="38">
+        <v>10</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7">
-        <v>22</v>
-      </c>
-      <c r="H7" s="30">
-        <v>43984</v>
-      </c>
-      <c r="I7">
-        <v>22</v>
-      </c>
-      <c r="J7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>43984</v>
-      </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="E8">
-        <v>75</v>
-      </c>
-      <c r="H8" s="30">
-        <v>43984</v>
-      </c>
-      <c r="I8">
-        <v>75</v>
-      </c>
-      <c r="J8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>43985</v>
-      </c>
-      <c r="C9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="E9">
-        <v>85</v>
-      </c>
-      <c r="H9" s="30">
-        <v>43985</v>
-      </c>
-      <c r="I9">
-        <v>85</v>
-      </c>
-      <c r="J9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>43985</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E10">
-        <v>33</v>
-      </c>
-      <c r="H10" s="30">
-        <v>43985</v>
-      </c>
-      <c r="I10">
-        <v>33</v>
-      </c>
-      <c r="J10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>43986</v>
-      </c>
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="E11">
-        <v>44</v>
-      </c>
-      <c r="H11" s="30">
-        <v>43986</v>
-      </c>
-      <c r="I11">
-        <v>44</v>
-      </c>
-      <c r="J11" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>43994</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="E12">
-        <v>-1000</v>
-      </c>
-      <c r="H12" s="30">
-        <v>43994</v>
-      </c>
-      <c r="I12">
-        <v>-1000</v>
-      </c>
-      <c r="J12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="38" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>43982</v>
-      </c>
-      <c r="B14" s="38">
-        <v>10</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>43983</v>
-      </c>
-      <c r="B15" s="38">
-        <v>11</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>43985</v>
-      </c>
-      <c r="B16" s="38">
-        <v>33</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>134</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2927,16 +2447,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A79CC3C-10DD-4C9D-955D-781259440CED}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2:H4"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2.140625" customWidth="1"/>
     <col min="4" max="4" width="30.85546875" style="12" bestFit="1" customWidth="1"/>
@@ -3036,197 +2556,43 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5"/>
+      <c r="A5" s="5">
+        <v>44015</v>
+      </c>
+      <c r="B5" s="37"/>
+      <c r="C5" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="50">
+        <v>95</v>
+      </c>
+      <c r="H5" s="5">
+        <v>44015</v>
+      </c>
+      <c r="I5">
+        <v>95</v>
+      </c>
+      <c r="J5" s="51" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>43983</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="E6">
-        <v>95</v>
-      </c>
-      <c r="H6" s="30">
-        <v>43983</v>
-      </c>
-      <c r="I6">
-        <v>95</v>
-      </c>
-      <c r="J6" t="s">
-        <v>136</v>
+      <c r="B6" s="38" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>43984</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
+        <v>43982</v>
+      </c>
+      <c r="B7" s="38">
+        <v>10</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="E7">
-        <v>66</v>
-      </c>
-      <c r="H7" s="30">
-        <v>43984</v>
-      </c>
-      <c r="I7">
-        <v>66</v>
-      </c>
-      <c r="J7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>43984</v>
-      </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="E8">
-        <v>105</v>
-      </c>
-      <c r="H8" s="30">
-        <v>43984</v>
-      </c>
-      <c r="I8">
-        <v>105</v>
-      </c>
-      <c r="J8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>43985</v>
-      </c>
-      <c r="C9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="E9">
-        <v>77</v>
-      </c>
-      <c r="H9" s="30">
-        <v>43986</v>
-      </c>
-      <c r="I9">
-        <v>77</v>
-      </c>
-      <c r="J9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>43985</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="E10">
-        <v>115</v>
-      </c>
-      <c r="H10" s="30">
-        <v>43985</v>
-      </c>
-      <c r="I10">
-        <v>115</v>
-      </c>
-      <c r="J10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>43987</v>
-      </c>
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="E11">
-        <v>88</v>
-      </c>
-      <c r="H11" s="30">
-        <v>43987</v>
-      </c>
-      <c r="I11">
-        <v>88</v>
-      </c>
-      <c r="J11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>43995</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="E12">
-        <v>-2000</v>
-      </c>
-      <c r="H12" s="30">
-        <v>43995</v>
-      </c>
-      <c r="I12">
-        <v>-2000</v>
-      </c>
-      <c r="J12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="38" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>43982</v>
-      </c>
-      <c r="B14" s="38">
-        <v>10</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>43983</v>
-      </c>
-      <c r="B15" s="38">
-        <v>55</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>146</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3812,7 +3178,7 @@
         <v>-1000</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3823,7 +3189,7 @@
         <v>-1000</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3843,7 +3209,7 @@
         <v>-2000</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Write spends & groceries to Expected Out
</commit_message>
<xml_diff>
--- a/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
+++ b/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\Reconciliate\reconciliation-samples\For-debugging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDE57F7-67E9-480F-853B-0D25BD636C10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7E0FE0-33AC-48E7-A34B-BF7E2AA31783}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24090" yWindow="630" windowWidth="18525" windowHeight="12285" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="2" activeTab="10" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank In" sheetId="7" r:id="rId1"/>
@@ -241,7 +241,7 @@
     <definedName name="VATRateToHMRC" localSheetId="3">#REF!</definedName>
     <definedName name="VATRateToHMRC">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -259,7 +259,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="146">
   <si>
     <t>notes</t>
   </si>
@@ -366,21 +366,9 @@
     <t>NOTES 007</t>
   </si>
   <si>
-    <t>NOTES 008</t>
-  </si>
-  <si>
-    <t>NOTES 009</t>
-  </si>
-  <si>
-    <t>NOTES 010</t>
-  </si>
-  <si>
     <t>NOTES 011</t>
   </si>
   <si>
-    <t>NOTES 012</t>
-  </si>
-  <si>
     <t>NOTES 013</t>
   </si>
   <si>
@@ -640,6 +628,75 @@
   </si>
   <si>
     <t>AmEx monthly transaction 01</t>
+  </si>
+  <si>
+    <t>NOTES 015</t>
+  </si>
+  <si>
+    <t>Code069</t>
+  </si>
+  <si>
+    <t>NOTES 069</t>
+  </si>
+  <si>
+    <t>Code078</t>
+  </si>
+  <si>
+    <t>Code076</t>
+  </si>
+  <si>
+    <t>Code079</t>
+  </si>
+  <si>
+    <t>NOTES 078</t>
+  </si>
+  <si>
+    <t>NOTES 076</t>
+  </si>
+  <si>
+    <t>NOTES 079</t>
+  </si>
+  <si>
+    <t>Expenses Weekly</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>£25.95 on 14/7/14, then £50.99 for 3 months, then £60.99 (plus calls)</t>
+  </si>
+  <si>
+    <t>Code074</t>
+  </si>
+  <si>
+    <t>Code075</t>
+  </si>
+  <si>
+    <t>Monthly expense 004</t>
+  </si>
+  <si>
+    <t>Monthly expense 005</t>
+  </si>
+  <si>
+    <t>Monthly expense 006</t>
+  </si>
+  <si>
+    <t>Monthly expense 007</t>
+  </si>
+  <si>
+    <t>Monthly expense 008</t>
+  </si>
+  <si>
+    <t>Monthly expense 009</t>
+  </si>
+  <si>
+    <t>Monthly expense 010</t>
+  </si>
+  <si>
+    <t>Monthly expense 011</t>
+  </si>
+  <si>
+    <t>Monthly expense 012</t>
   </si>
 </sst>
 </file>
@@ -652,7 +709,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -694,6 +751,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -719,7 +782,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -796,6 +859,10 @@
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1255,13 +1322,13 @@
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="37">
@@ -1277,10 +1344,10 @@
         <v>1000</v>
       </c>
       <c r="N2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="O2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1289,13 +1356,13 @@
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="13">
@@ -1311,10 +1378,10 @@
         <v>5</v>
       </c>
       <c r="N3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O3" t="s">
         <v>46</v>
-      </c>
-      <c r="O3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1323,13 +1390,13 @@
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="13">
@@ -1345,10 +1412,10 @@
         <v>10</v>
       </c>
       <c r="N4" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4" t="s">
         <v>46</v>
-      </c>
-      <c r="O4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1357,13 +1424,13 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F5" s="10">
         <v>12345</v>
@@ -1381,15 +1448,15 @@
         <v>15</v>
       </c>
       <c r="N5" t="s">
+        <v>42</v>
+      </c>
+      <c r="O5" t="s">
         <v>46</v>
-      </c>
-      <c r="O5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1400,10 +1467,10 @@
         <v>5.05</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1438,7 +1505,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D1" s="39"/>
       <c r="E1" s="34" t="s">
@@ -1467,7 +1534,7 @@
         <v>19</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="J2" s="20">
         <v>43616</v>
@@ -1492,7 +1559,7 @@
         <v>20</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="J3" s="20"/>
       <c r="K3" s="14">
@@ -1515,7 +1582,7 @@
         <v>19</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="K4" s="14">
         <v>3</v>
@@ -1523,7 +1590,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="48" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1533,16 +1600,16 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF22F54-1C2B-49C1-90A9-21044AC295B0}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
@@ -1570,16 +1637,16 @@
         <v>3</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H1" s="34"/>
       <c r="I1" s="34" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="34" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="17"/>
@@ -1600,7 +1667,7 @@
         <v>19</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="K3" s="20"/>
     </row>
@@ -1619,13 +1686,13 @@
         <v>20</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K4" s="20"/>
     </row>
     <row r="5" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B5" s="18">
         <f>$K$3+L5</f>
@@ -1638,368 +1705,686 @@
         <v>19</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="47">
-        <f>SUM(C3:C5)</f>
-        <v>45</v>
-      </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="19"/>
+      <c r="A6" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="37">
+        <v>10</v>
+      </c>
+      <c r="D6" s="37"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="16"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="19"/>
+      <c r="A7" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="37">
+        <v>10</v>
+      </c>
+      <c r="D7" s="37"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="19"/>
+      <c r="A8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="37">
+        <v>10</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="18">
-        <f>$K$9+L9</f>
-        <v>43617</v>
-      </c>
-      <c r="C9" s="17">
-        <v>35</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>19</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B9" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="37">
+        <v>10</v>
+      </c>
+      <c r="D9" s="37"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="K9" s="20">
-        <v>43616</v>
-      </c>
-      <c r="L9" s="14">
-        <v>1</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="18">
-        <f t="shared" ref="B10:B12" si="0">$K$9+L10</f>
-        <v>43618</v>
-      </c>
-      <c r="C10" s="17">
-        <v>45</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>20</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="B10" s="53"/>
+      <c r="C10" s="37">
+        <v>10</v>
+      </c>
+      <c r="D10" s="37"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="K10" s="20"/>
-      <c r="L10" s="14">
-        <v>2</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="B11" s="18">
-        <f t="shared" si="0"/>
-        <v>43619</v>
-      </c>
-      <c r="C11" s="17">
-        <v>55</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>19</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="B11" s="53"/>
+      <c r="C11" s="37">
+        <v>10</v>
+      </c>
+      <c r="D11" s="37"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="L11" s="14">
+        <v>142</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="53"/>
+      <c r="C12" s="37">
+        <v>10</v>
+      </c>
+      <c r="D12" s="37"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="53"/>
+      <c r="C13" s="37">
+        <v>10</v>
+      </c>
+      <c r="D13" s="37"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="37">
+        <v>10</v>
+      </c>
+      <c r="D14" s="37"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="47">
+        <f>SUM(C3:C14)</f>
+        <v>135</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="51"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="19"/>
+      <c r="K16" s="20">
+        <v>43616</v>
+      </c>
+      <c r="L16" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="51"/>
+      <c r="B17" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" s="37"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="19"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="37">
+        <v>10</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="19"/>
+      <c r="L18" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="B12" s="18">
-        <f t="shared" si="0"/>
-        <v>43620</v>
-      </c>
-      <c r="C12" s="17">
-        <v>1000</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="L12" s="14">
+    <row r="19" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="16"/>
+      <c r="C19" s="37">
+        <v>10</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="19"/>
+      <c r="L19" s="14">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B13" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="19"/>
-    </row>
-    <row r="14" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" s="18">
-        <f>$K$9+L14</f>
-        <v>43617</v>
-      </c>
-      <c r="C14" s="17">
-        <v>65</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="L14" s="14">
+    <row r="20" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="37">
+        <v>10</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="19"/>
+    </row>
+    <row r="21" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="37">
+        <v>10</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="19"/>
+      <c r="L21" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="18">
-        <f t="shared" ref="B15:B16" si="1">$K$9+L15</f>
-        <v>43618</v>
-      </c>
-      <c r="C15" s="17">
-        <v>75</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="L15" s="14">
+    <row r="22" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="37">
+        <v>10</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="19"/>
+      <c r="L22" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="B16" s="18">
-        <f t="shared" si="1"/>
-        <v>43619</v>
-      </c>
-      <c r="C16" s="17">
-        <v>85</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="L16" s="14">
+    <row r="23" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="37">
+        <v>10</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="19"/>
+      <c r="L23" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="B18" s="18">
-        <f>$K$9+L18</f>
-        <v>43617</v>
-      </c>
-      <c r="C18" s="17">
-        <v>95</v>
-      </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="B19" s="18">
-        <f t="shared" ref="B19:B20" si="2">$K$9+L19</f>
-        <v>43618</v>
-      </c>
-      <c r="C19" s="17">
-        <v>105</v>
-      </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="B20" s="18">
-        <f t="shared" si="2"/>
-        <v>43619</v>
-      </c>
-      <c r="C20" s="17">
-        <v>115</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="12">
-        <f>SUM(C9:C20)</f>
-        <v>1675</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="34" t="s">
-        <v>78</v>
-      </c>
-    </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B24" s="18">
-        <v>43466</v>
-      </c>
-      <c r="C24" s="17">
-        <v>125</v>
-      </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>99</v>
-      </c>
+      <c r="A24" s="14"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="19"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="14"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" s="18">
-        <v>43647</v>
-      </c>
-      <c r="C25" s="17">
-        <v>135</v>
-      </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>100</v>
-      </c>
+      <c r="A25" s="14"/>
+      <c r="B25" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="19"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
       <c r="K25" s="20"/>
-      <c r="L25" s="14"/>
+      <c r="L25" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B26" s="18">
-        <v>43770</v>
+        <f>$K$16+L16</f>
+        <v>43617</v>
       </c>
       <c r="C26" s="17">
-        <v>145</v>
+        <v>35</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="19" t="s">
         <v>19</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="46" t="s">
+      <c r="A27" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="18">
+        <f t="shared" ref="B27:B29" si="0">$K$16+L17</f>
+        <v>43618</v>
+      </c>
+      <c r="C27" s="17">
+        <v>45</v>
+      </c>
+      <c r="D27" s="14"/>
+      <c r="E27" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="18">
+        <f t="shared" si="0"/>
+        <v>43619</v>
+      </c>
+      <c r="C28" s="17">
+        <v>55</v>
+      </c>
+      <c r="D28" s="14"/>
+      <c r="E28" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" s="18">
+        <f t="shared" si="0"/>
+        <v>43620</v>
+      </c>
+      <c r="C29" s="17">
+        <v>1000</v>
+      </c>
+      <c r="D29" s="14"/>
+      <c r="E29" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="18">
+        <f>$K$16+L21</f>
+        <v>43617</v>
+      </c>
+      <c r="C31" s="17">
+        <v>65</v>
+      </c>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="12">
-        <f>SUM(C24:C26)</f>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="14"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="18">
+        <f t="shared" ref="B32:B33" si="1">$K$16+L22</f>
+        <v>43618</v>
+      </c>
+      <c r="C32" s="17">
+        <v>75</v>
+      </c>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="14"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="18">
+        <f t="shared" si="1"/>
+        <v>43619</v>
+      </c>
+      <c r="C33" s="17">
+        <v>85</v>
+      </c>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="G34" s="14"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="18">
+        <f>$K$16+L25</f>
+        <v>43617</v>
+      </c>
+      <c r="C35" s="17">
+        <v>95</v>
+      </c>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="18">
+        <f t="shared" ref="B36:B37" si="2">$K$16+L26</f>
+        <v>43618</v>
+      </c>
+      <c r="C36" s="17">
+        <v>105</v>
+      </c>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="18">
+        <f t="shared" si="2"/>
+        <v>43619</v>
+      </c>
+      <c r="C37" s="17">
+        <v>115</v>
+      </c>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="12">
+        <f>SUM(C26:C37)</f>
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" s="18">
+        <v>43466</v>
+      </c>
+      <c r="C41" s="17">
+        <v>125</v>
+      </c>
+      <c r="D41" s="14"/>
+      <c r="E41" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="18">
+        <v>43647</v>
+      </c>
+      <c r="C42" s="17">
+        <v>135</v>
+      </c>
+      <c r="D42" s="14"/>
+      <c r="E42" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" s="18">
+        <v>43770</v>
+      </c>
+      <c r="C43" s="17">
+        <v>145</v>
+      </c>
+      <c r="D43" s="14"/>
+      <c r="E43" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="12">
+        <f>SUM(C41:C43)</f>
         <v>405</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2052,13 +2437,13 @@
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="13">
@@ -2075,10 +2460,10 @@
         <v>5</v>
       </c>
       <c r="N2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" t="s">
         <v>46</v>
-      </c>
-      <c r="O2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -2087,13 +2472,13 @@
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="13">
@@ -2110,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="N3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O3" t="s">
         <v>46</v>
-      </c>
-      <c r="O3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -2122,13 +2507,13 @@
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F4" s="10">
         <v>12345</v>
@@ -2147,10 +2532,10 @@
         <v>15</v>
       </c>
       <c r="N4" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4" t="s">
         <v>46</v>
-      </c>
-      <c r="O4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -2159,13 +2544,13 @@
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="13">
@@ -2182,10 +2567,10 @@
         <v>35</v>
       </c>
       <c r="N5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2194,13 +2579,13 @@
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="13">
@@ -2217,10 +2602,10 @@
         <v>500</v>
       </c>
       <c r="N6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -2229,13 +2614,13 @@
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="13">
@@ -2252,10 +2637,10 @@
         <v>1500</v>
       </c>
       <c r="N7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2272,10 +2657,10 @@
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="13"/>
@@ -2314,14 +2699,14 @@
         <v>1</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C1" s="33"/>
       <c r="D1" s="34" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F1" s="34" t="s">
         <v>22</v>
@@ -2333,10 +2718,10 @@
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E2" s="13">
         <v>5</v>
@@ -2348,7 +2733,7 @@
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2357,10 +2742,10 @@
       </c>
       <c r="B3" s="37"/>
       <c r="C3" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E3" s="13">
         <v>10</v>
@@ -2372,7 +2757,7 @@
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2381,10 +2766,10 @@
       </c>
       <c r="B4" s="37"/>
       <c r="C4" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E4" s="13">
         <v>15</v>
@@ -2396,7 +2781,7 @@
         <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2405,10 +2790,10 @@
       </c>
       <c r="B5" s="37"/>
       <c r="C5" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E5" s="50">
         <v>65</v>
@@ -2420,12 +2805,12 @@
         <v>65</v>
       </c>
       <c r="J5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="38" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2436,7 +2821,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2449,7 +2834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A79CC3C-10DD-4C9D-955D-781259440CED}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
@@ -2470,14 +2855,14 @@
         <v>1</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C1" s="33"/>
       <c r="D1" s="34" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F1" s="34" t="s">
         <v>22</v>
@@ -2489,10 +2874,10 @@
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E2" s="13">
         <v>5</v>
@@ -2504,7 +2889,7 @@
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2513,10 +2898,10 @@
       </c>
       <c r="B3" s="37"/>
       <c r="C3" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E3" s="13">
         <v>10</v>
@@ -2528,7 +2913,7 @@
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2537,10 +2922,10 @@
       </c>
       <c r="B4" s="37"/>
       <c r="C4" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E4" s="13">
         <v>15</v>
@@ -2552,7 +2937,7 @@
         <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2561,10 +2946,10 @@
       </c>
       <c r="B5" s="37"/>
       <c r="C5" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E5" s="50">
         <v>95</v>
@@ -2576,12 +2961,12 @@
         <v>95</v>
       </c>
       <c r="J5" s="51" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="38" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2592,7 +2977,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2626,19 +3011,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C1" s="34" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G1" s="34" t="s">
         <v>3</v>
@@ -2662,7 +3047,7 @@
         <v>43952</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2682,7 +3067,7 @@
         <v>25</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2702,7 +3087,7 @@
         <v>25</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2718,13 +3103,13 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E6" s="49">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2735,13 +3120,13 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E7" s="49">
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2752,13 +3137,13 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E8" s="49">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2768,11 +3153,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB17BBD-6FBB-4BDC-8FD6-599D29D94644}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2788,8 +3173,8 @@
         <v>21</v>
       </c>
       <c r="B1" s="22">
-        <f>SUM(B2:B287)</f>
-        <v>9665.7950000000001</v>
+        <f>SUM(B2:B293)</f>
+        <v>9875.7950000000001</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23" t="s">
@@ -2917,7 +3302,7 @@
       </c>
       <c r="C9" s="26"/>
       <c r="D9" s="28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E9" s="27"/>
       <c r="F9" s="26"/>
@@ -2949,7 +3334,7 @@
       </c>
       <c r="C11" s="26"/>
       <c r="D11" s="28" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="26"/>
@@ -2958,47 +3343,49 @@
       <c r="I11" s="26"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
+      <c r="A12" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="25">
+        <v>10</v>
+      </c>
+      <c r="C12" s="26"/>
+      <c r="D12" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="27"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="27">
-        <v>10</v>
+        <v>83</v>
+      </c>
+      <c r="B13" s="25">
+        <v>20</v>
       </c>
       <c r="C13" s="26"/>
       <c r="D13" s="28" t="s">
-        <v>37</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="26"/>
       <c r="G13" s="26"/>
       <c r="H13" s="26"/>
       <c r="I13" s="26"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>16</v>
+        <v>126</v>
       </c>
       <c r="B14" s="25">
-        <v>102.884</v>
+        <v>30</v>
       </c>
       <c r="C14" s="26"/>
       <c r="D14" s="28" t="s">
-        <v>36</v>
+        <v>129</v>
       </c>
       <c r="E14" s="27"/>
       <c r="F14" s="26"/>
@@ -3007,105 +3394,204 @@
       <c r="I14" s="26"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
+      <c r="A15" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="25">
+        <v>40</v>
+      </c>
+      <c r="C15" s="26"/>
+      <c r="D15" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="27"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>17</v>
+        <v>127</v>
       </c>
       <c r="B16" s="25">
-        <v>1799.2239999999999</v>
-      </c>
-      <c r="C16" s="23"/>
+        <v>50</v>
+      </c>
+      <c r="C16" s="26"/>
       <c r="D16" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
+        <v>130</v>
+      </c>
+      <c r="E16" s="27"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="25">
-        <v>499.82400000000001</v>
-      </c>
-      <c r="C17" s="23"/>
+        <v>128</v>
+      </c>
+      <c r="B17" s="52">
+        <v>60</v>
+      </c>
       <c r="D17" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
+        <v>131</v>
+      </c>
+      <c r="E17" s="27"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="25">
-        <v>1265.2239999999999</v>
-      </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="24"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="25">
-        <v>2633.3320000000003</v>
+      <c r="B19" s="27">
+        <v>10</v>
       </c>
       <c r="C19" s="26"/>
       <c r="D19" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="26"/>
+        <v>35</v>
+      </c>
       <c r="G19" s="26"/>
       <c r="H19" s="26"/>
       <c r="I19" s="26"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25">
-        <f>SUM(B19:B19)</f>
-        <v>2633.3320000000003</v>
-      </c>
+      <c r="A20" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="25">
+        <v>102.884</v>
+      </c>
+      <c r="C20" s="26"/>
       <c r="D20" s="28" t="s">
-        <v>42</v>
+        <v>123</v>
       </c>
       <c r="E20" s="27"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
       <c r="H20" s="26"/>
       <c r="I20" s="26"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="24"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="25">
+        <v>1799.2239999999999</v>
+      </c>
+      <c r="C22" s="23"/>
+      <c r="D22" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="E22" s="24"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="25">
+        <v>499.82400000000001</v>
+      </c>
+      <c r="C23" s="23"/>
+      <c r="D23" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="24"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="25">
+        <v>1265.2239999999999</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="27"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="25">
+        <v>2633.3320000000003</v>
+      </c>
+      <c r="C25" s="26"/>
+      <c r="D25" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="27"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25">
+        <f>SUM(B25:B25)</f>
+        <v>2633.3320000000003</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="27"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3143,12 +3629,12 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B2" s="40"/>
       <c r="C2" s="7"/>
       <c r="D2" s="34" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="7"/>
@@ -3163,38 +3649,38 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B4" s="40">
         <v>1000</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E4" s="13">
         <v>-1000</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D5" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E5" s="13">
         <v>-1000</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E6" s="13">
         <v>-1000</v>
@@ -3203,13 +3689,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E7" s="13">
         <v>-2000</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -3240,14 +3726,14 @@
         <v>1</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C1" s="33"/>
       <c r="D1" s="34" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F1" s="34" t="s">
         <v>22</v>
@@ -3259,10 +3745,10 @@
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E2" s="37">
         <v>5</v>
@@ -3274,10 +3760,10 @@
       </c>
       <c r="B3" s="37"/>
       <c r="C3" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E3" s="37">
         <v>10</v>
@@ -3289,10 +3775,10 @@
       </c>
       <c r="B4" s="37"/>
       <c r="C4" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E4" s="37">
         <v>15</v>
@@ -3306,7 +3792,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3334,7 +3820,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C1" s="42" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Update CHB text as well as amount
</commit_message>
<xml_diff>
--- a/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
+++ b/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\Reconciliate\reconciliation-samples\For-debugging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD169BE1-9063-445C-971A-787FEACAE0B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81B3CFF-DC76-4A3A-83CE-32DC4DDCD0CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="2" activeTab="5" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
@@ -259,7 +259,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="148">
   <si>
     <t>notes</t>
   </si>
@@ -700,6 +700,9 @@
   </si>
   <si>
     <t>Ad Hoc amounts</t>
+  </si>
+  <si>
+    <t>CHB owed (Apr to Jun 2020)</t>
   </si>
 </sst>
 </file>
@@ -3175,7 +3178,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3553,7 +3556,7 @@
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="28" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="23"/>

</xml_diff>

<commit_message>
Pull in bank transactions from Ex In as well as expense transactions.
</commit_message>
<xml_diff>
--- a/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
+++ b/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\Reconciliate\reconciliation-samples\For-debugging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81B3CFF-DC76-4A3A-83CE-32DC4DDCD0CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F296DFB-3956-4DD1-B1B0-EA75CA77B168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="2" activeTab="5" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="3285" yWindow="75" windowWidth="18705" windowHeight="12720" firstSheet="2" activeTab="4" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank In" sheetId="7" r:id="rId1"/>
@@ -259,7 +259,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="150">
   <si>
     <t>notes</t>
   </si>
@@ -703,6 +703,12 @@
   </si>
   <si>
     <t>CHB owed (Apr to Jun 2020)</t>
+  </si>
+  <si>
+    <t>Bank Transaction</t>
+  </si>
+  <si>
+    <t>bank transaction from Expected In</t>
   </si>
 </sst>
 </file>
@@ -3009,11 +3015,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D16E861-33A2-4129-91DA-2BF02F143AFA}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E4"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3022,9 +3028,9 @@
     <col min="2" max="2" width="18.42578125" style="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="34" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -3165,6 +3171,23 @@
       </c>
       <c r="G8" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="30">
+        <v>43986</v>
+      </c>
+      <c r="B9" s="38">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E9" s="49">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -3176,7 +3199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB17BBD-6FBB-4BDC-8FD6-599D29D94644}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>

</xml_diff>

<commit_message>
Fix test data for testing Bank transactions on Ex In
</commit_message>
<xml_diff>
--- a/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
+++ b/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\Reconciliate\reconciliation-samples\For-debugging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F296DFB-3956-4DD1-B1B0-EA75CA77B168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AB373E-C68F-4E64-9E29-027445495461}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="75" windowWidth="18705" windowHeight="12720" firstSheet="2" activeTab="4" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="24330" yWindow="1050" windowWidth="18705" windowHeight="12720" firstSheet="2" activeTab="4" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank In" sheetId="7" r:id="rId1"/>
@@ -3019,14 +3019,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" style="38" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="38" bestFit="1" customWidth="1"/>
@@ -3178,7 +3178,7 @@
         <v>43986</v>
       </c>
       <c r="B9" s="38">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="C9" t="s">
         <v>148</v>

</xml_diff>

<commit_message>
Update num months as well as end date for CHB text.
</commit_message>
<xml_diff>
--- a/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
+++ b/reconciliation-samples/For-debugging/Your-Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\Reconciliate\reconciliation-samples\For-debugging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AB373E-C68F-4E64-9E29-027445495461}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EEC626-5E48-4D10-847E-E218B27AECB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24330" yWindow="1050" windowWidth="18705" windowHeight="12720" firstSheet="2" activeTab="4" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="18705" windowHeight="12720" firstSheet="2" activeTab="5" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank In" sheetId="7" r:id="rId1"/>
@@ -702,13 +702,13 @@
     <t>Ad Hoc amounts</t>
   </si>
   <si>
-    <t>CHB owed (Apr to Jun 2020)</t>
-  </si>
-  <si>
     <t>Bank Transaction</t>
   </si>
   <si>
     <t>bank transaction from Expected In</t>
+  </si>
+  <si>
+    <t>CHB owed (this is 16 months Apr 2019 to Jul 2020)</t>
   </si>
 </sst>
 </file>
@@ -3017,7 +3017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D16E861-33A2-4129-91DA-2BF02F143AFA}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
@@ -3181,13 +3181,13 @@
         <v>150</v>
       </c>
       <c r="C9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E9" s="49">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3199,16 +3199,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB17BBD-6FBB-4BDC-8FD6-599D29D94644}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3579,7 +3579,7 @@
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="28" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="23"/>

</xml_diff>